<commit_message>
make pdf work again
</commit_message>
<xml_diff>
--- a/registration.xlsx
+++ b/registration.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schins\Documents\AFROTC\Drill Meet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schins\Desktop\RPI DRILL MEET GIT KRACKEN\rpidrillmeet.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0124509A-1997-408D-9702-67D060A56FF8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25130" windowHeight="12330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25130" windowHeight="12330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
     <sheet name="Registration" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Name of School:</t>
   </si>
@@ -200,12 +201,18 @@
   </si>
   <si>
     <t>✝Registration Discount (15%)</t>
+  </si>
+  <si>
+    <t>$13 online</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$17 Day of </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -627,19 +634,22 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -647,6 +657,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -663,14 +676,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -711,7 +718,13 @@
     <xdr:ext cx="7296150" cy="9229725"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="2" name="image3.png" title="Image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -744,7 +757,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -782,7 +801,13 @@
     <xdr:ext cx="2571750" cy="2505075"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image1.jpg" descr="Watermarked big"/>
+        <xdr:cNvPr id="2" name="image1.jpg" descr="Watermarked big">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -810,7 +835,13 @@
     <xdr:ext cx="2457450" cy="2514600"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="image2.jpg" descr="Watermarked big"/>
+        <xdr:cNvPr id="3" name="image2.jpg" descr="Watermarked big">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -843,7 +874,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -887,7 +924,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1181,7 +1224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A21:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2181,11 +2224,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2199,22 +2242,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:5" ht="23" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -2234,55 +2277,55 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="39"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="23"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="41" t="s">
@@ -2307,19 +2350,19 @@
       <c r="E10" s="46"/>
     </row>
     <row r="11" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
     </row>
     <row r="12" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="23"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="6">
         <v>60</v>
       </c>
@@ -2330,10 +2373,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="23"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="6">
         <v>60</v>
       </c>
@@ -2344,19 +2387,19 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="6">
         <v>10</v>
       </c>
@@ -2367,10 +2410,10 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="6">
         <v>45</v>
       </c>
@@ -2381,10 +2424,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="6">
         <v>30</v>
       </c>
@@ -2395,19 +2438,19 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
     </row>
     <row r="19" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="9">
         <v>50</v>
       </c>
@@ -2418,10 +2461,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="23"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="9">
         <v>40</v>
       </c>
@@ -2432,10 +2475,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="23"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="9">
         <v>20</v>
       </c>
@@ -2446,10 +2489,10 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="9">
         <v>20</v>
       </c>
@@ -2460,19 +2503,19 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="23"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="6">
         <v>40</v>
       </c>
@@ -2483,19 +2526,19 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
     </row>
     <row r="26" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="6">
         <v>40</v>
       </c>
@@ -2506,10 +2549,10 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="23"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="6">
         <v>25</v>
       </c>
@@ -2520,10 +2563,10 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="23"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="6">
         <v>25</v>
       </c>
@@ -2534,10 +2577,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="23"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="6">
         <v>25</v>
       </c>
@@ -2548,10 +2591,10 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="23"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="6">
         <v>15</v>
       </c>
@@ -2562,10 +2605,10 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="23"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="6">
         <v>25</v>
       </c>
@@ -2576,10 +2619,10 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="23"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="6">
         <v>25</v>
       </c>
@@ -2590,10 +2633,10 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="23"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="6">
         <v>25</v>
       </c>
@@ -2604,10 +2647,10 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="23"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="6">
         <v>25</v>
       </c>
@@ -2618,10 +2661,10 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="23"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="10">
         <v>10</v>
       </c>
@@ -2631,19 +2674,19 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="31"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="23"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="24"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11"/>
       <c r="B37" s="12"/>
-      <c r="C37" s="38" t="s">
+      <c r="C37" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="23"/>
+      <c r="D37" s="24"/>
       <c r="E37" s="13">
         <f>SUM(E12:E35)</f>
         <v>10</v>
@@ -2652,10 +2695,10 @@
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11"/>
       <c r="B38" s="12"/>
-      <c r="C38" s="32" t="s">
+      <c r="C38" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="23"/>
+      <c r="D38" s="24"/>
       <c r="E38" s="14">
         <f>B56</f>
         <v>0</v>
@@ -2664,10 +2707,10 @@
     <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="11"/>
       <c r="B39" s="12"/>
-      <c r="C39" s="32" t="s">
+      <c r="C39" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="23"/>
+      <c r="D39" s="24"/>
       <c r="E39" s="14" t="s">
         <v>45</v>
       </c>
@@ -2675,41 +2718,41 @@
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="15"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="33" t="s">
+      <c r="C40" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="23"/>
+      <c r="D40" s="24"/>
       <c r="E40" s="14">
         <f>E37+E38</f>
         <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="36"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="30"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="30"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="31"/>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2718,8 +2761,15 @@
       <c r="A47" s="17" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="50" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="18" t="s">
@@ -3714,19 +3764,24 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
     <mergeCell ref="A43:E43"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="A19:B19"/>
@@ -3743,24 +3798,19 @@
     <mergeCell ref="A42:E42"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
huge drill file update
</commit_message>
<xml_diff>
--- a/registration.xlsx
+++ b/registration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schins\Desktop\RPI DRILL MEET GIT KRACKEN\rpidrillmeet.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0A289E-61E0-4233-A1A7-1D373A61D7AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB56E2D-F8E8-4718-A592-6D21B511D3D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -641,39 +641,32 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -690,12 +683,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2249,22 +2249,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2284,92 +2284,92 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="26" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="23"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="33" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="45" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
+      <c r="A10" s="43"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="23"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="6">
         <v>60</v>
       </c>
@@ -2380,10 +2380,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="23"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="6">
         <v>60</v>
       </c>
@@ -2394,19 +2394,19 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="6">
         <v>10</v>
       </c>
@@ -2417,10 +2417,10 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="6">
         <v>45</v>
       </c>
@@ -2431,10 +2431,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="6">
         <v>30</v>
       </c>
@@ -2445,19 +2445,19 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="9">
         <v>50</v>
       </c>
@@ -2468,10 +2468,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="23"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="9">
         <v>40</v>
       </c>
@@ -2482,10 +2482,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="23"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="9">
         <v>20</v>
       </c>
@@ -2496,10 +2496,10 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="9">
         <v>20</v>
       </c>
@@ -2510,19 +2510,19 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28" t="s">
+      <c r="A23" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="23"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="6">
         <v>40</v>
       </c>
@@ -2533,19 +2533,19 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
     </row>
     <row r="26" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="6">
         <v>40</v>
       </c>
@@ -2556,10 +2556,10 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="23"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="6">
         <v>25</v>
       </c>
@@ -2570,10 +2570,10 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="23"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="6">
         <v>25</v>
       </c>
@@ -2584,10 +2584,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="23"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="6">
         <v>25</v>
       </c>
@@ -2598,10 +2598,10 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="23"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="6">
         <v>15</v>
       </c>
@@ -2612,10 +2612,10 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="23"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="6">
         <v>25</v>
       </c>
@@ -2626,10 +2626,10 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="23"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="6">
         <v>25</v>
       </c>
@@ -2640,10 +2640,10 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="23"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="6">
         <v>25</v>
       </c>
@@ -2654,10 +2654,10 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="23"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="6">
         <v>25</v>
       </c>
@@ -2668,10 +2668,10 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="23"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="10">
         <v>10</v>
       </c>
@@ -2681,19 +2681,19 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="38"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="23"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="24"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="12"/>
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="23"/>
+      <c r="D37" s="24"/>
       <c r="E37" s="13">
         <f>SUM(E12:E35)</f>
         <v>10</v>
@@ -2702,10 +2702,10 @@
     <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="12"/>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="23"/>
+      <c r="D38" s="24"/>
       <c r="E38" s="14">
         <f>B56</f>
         <v>0</v>
@@ -2714,10 +2714,10 @@
     <row r="39" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="12"/>
-      <c r="C39" s="39" t="s">
+      <c r="C39" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D39" s="23"/>
+      <c r="D39" s="24"/>
       <c r="E39" s="14" t="s">
         <v>45</v>
       </c>
@@ -2725,41 +2725,41 @@
     <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15"/>
       <c r="B40" s="16"/>
-      <c r="C40" s="40" t="s">
+      <c r="C40" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="23"/>
+      <c r="D40" s="24"/>
       <c r="E40" s="14">
         <f>E37+E38</f>
         <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="41" t="s">
+      <c r="A41" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="42"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="43"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="37"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="35" t="s">
+      <c r="A43" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="37"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="31"/>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3771,19 +3771,24 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
     <mergeCell ref="A43:E43"/>
     <mergeCell ref="A36:E36"/>
     <mergeCell ref="A19:B19"/>
@@ -3800,24 +3805,19 @@
     <mergeCell ref="A42:E42"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="A8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>